<commit_message>
Added DDL library, 5digitTimeStamp, update catch block, allUTILS package
</commit_message>
<xml_diff>
--- a/Data Files All/Book1.xlsx
+++ b/Data Files All/Book1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
   <si>
     <t>userName</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Blank26</t>
+  </si>
+  <si>
+    <t>Blank000</t>
+  </si>
+  <si>
+    <t>Blank001</t>
   </si>
 </sst>
 </file>
@@ -447,10 +453,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added pdf file reader demo
</commit_message>
<xml_diff>
--- a/Data Files All/Book1.xlsx
+++ b/Data Files All/Book1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
   <si>
     <t>userName</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Blank001</t>
+  </si>
+  <si>
+    <t>test54un</t>
+  </si>
+  <si>
+    <t>test54pw</t>
   </si>
 </sst>
 </file>
@@ -453,10 +459,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>